<commit_message>
change pw for pf
</commit_message>
<xml_diff>
--- a/S17/_members (2026).xlsx
+++ b/S17/_members (2026).xlsx
@@ -1081,7 +1081,7 @@
     <t xml:space="preserve">Pierre Fallot</t>
   </si>
   <si>
-    <t xml:space="preserve">012746</t>
+    <t xml:space="preserve">012745</t>
   </si>
   <si>
     <t xml:space="preserve">pfallot</t>
@@ -1445,11 +1445,11 @@
   <dimension ref="A1:V92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D86" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A86" activeCellId="0" sqref="A86"/>
+      <selection pane="bottomRight" activeCell="E88" activeCellId="0" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3661,7 +3661,7 @@
       </c>
       <c r="G85" s="5" t="str">
         <f aca="true">TEXT(TRUNC(1000000*RAND()),"000000")</f>
-        <v>544788</v>
+        <v>252476</v>
       </c>
       <c r="H85" s="8" t="s">
         <v>347</v>

</xml_diff>

<commit_message>
add admin to gent 2026
</commit_message>
<xml_diff>
--- a/S17/_members (2026).xlsx
+++ b/S17/_members (2026).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="370">
   <si>
     <t xml:space="preserve">Role</t>
   </si>
@@ -1121,6 +1121,15 @@
   </si>
   <si>
     <t xml:space="preserve">ksaidi04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karine Mitais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">206977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kmitais</t>
   </si>
 </sst>
 </file>
@@ -1442,14 +1451,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V92"/>
+  <dimension ref="A1:V93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D83" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A86" activeCellId="0" sqref="A86"/>
-      <selection pane="bottomRight" activeCell="E88" activeCellId="0" sqref="E88"/>
+      <selection pane="bottomLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
+      <selection pane="bottomRight" activeCell="C93" activeCellId="0" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3661,7 +3670,7 @@
       </c>
       <c r="G85" s="5" t="str">
         <f aca="true">TEXT(TRUNC(1000000*RAND()),"000000")</f>
-        <v>252476</v>
+        <v>284901</v>
       </c>
       <c r="H85" s="8" t="s">
         <v>347</v>
@@ -3769,6 +3778,20 @@
       </c>
       <c r="F92" s="1" t="s">
         <v>366</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pfallot is admin2 for S17
</commit_message>
<xml_diff>
--- a/S17/_members (2026).xlsx
+++ b/S17/_members (2026).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="371">
   <si>
     <t xml:space="preserve">Role</t>
   </si>
@@ -1085,6 +1085,9 @@
   </si>
   <si>
     <t xml:space="preserve">pfallot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">665736</t>
   </si>
   <si>
     <t xml:space="preserve">Anne-Chantal Drain</t>
@@ -1451,14 +1454,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V93"/>
+  <dimension ref="A1:V94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D83" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
-      <selection pane="bottomRight" activeCell="C93" activeCellId="0" sqref="C93"/>
+      <selection pane="bottomRight" activeCell="B94" activeCellId="0" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3670,7 +3673,7 @@
       </c>
       <c r="G85" s="5" t="str">
         <f aca="true">TEXT(TRUNC(1000000*RAND()),"000000")</f>
-        <v>284901</v>
+        <v>018451</v>
       </c>
       <c r="H85" s="8" t="s">
         <v>347</v>
@@ -3698,7 +3701,7 @@
         <v>343</v>
       </c>
       <c r="B87" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>344</v>
@@ -3714,6 +3717,9 @@
       <c r="A88" s="1" t="s">
         <v>348</v>
       </c>
+      <c r="B88" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="C88" s="1" t="s">
         <v>352</v>
       </c>
@@ -3726,72 +3732,105 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>348</v>
+        <v>343</v>
+      </c>
+      <c r="B89" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="C89" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E89" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="E89" s="5" t="s">
-        <v>356</v>
-      </c>
       <c r="F89" s="1" t="s">
-        <v>357</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="G89" s="5"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>348</v>
       </c>
+      <c r="B90" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="C90" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="F90" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>348</v>
       </c>
+      <c r="B91" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="C91" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="F91" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>348</v>
       </c>
+      <c r="B92" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="C92" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="F92" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>348</v>
       </c>
+      <c r="B93" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="C93" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="E93" s="5" t="s">
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B94" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="F93" s="1" t="s">
+      <c r="E94" s="5" t="s">
         <v>369</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>